<commit_message>
USD STD YC - disable invalid futures quotes
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/USD_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/USD_YCSTDBootstrapping.xlsx
@@ -1060,7 +1060,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1118,6 +1118,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="13"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1589,7 +1595,7 @@
     <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="227">
+  <cellXfs count="228">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -2099,6 +2105,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="4"/>
@@ -2801,7 +2810,7 @@
         <v>96</v>
       </c>
       <c r="D11" s="83">
-        <v>41655.504004629627</v>
+        <v>41655.505347222221</v>
       </c>
       <c r="E11" s="60"/>
       <c r="F11" s="59"/>
@@ -2917,7 +2926,7 @@
       </c>
       <c r="D14" s="80" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_USDYCSTD#0000</v>
+        <v>_USDYCSTD#0004</v>
       </c>
       <c r="E14" s="60"/>
       <c r="F14" s="59"/>
@@ -3287,9 +3296,9 @@
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
         <v>41655</v>
       </c>
-      <c r="D23" s="66" t="e">
+      <c r="D23" s="66">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
-        <v>#NUM!</v>
+        <v>3.7621420499449887E-2</v>
       </c>
       <c r="E23" s="60"/>
       <c r="F23" s="59"/>
@@ -3332,9 +3341,9 @@
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
         <v>59922</v>
       </c>
-      <c r="D24" s="64" t="e">
+      <c r="D24" s="64">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>#NUM!</v>
+        <v>1.4860692167494509E-3</v>
       </c>
       <c r="E24" s="60"/>
       <c r="F24" s="59"/>
@@ -3377,8 +3386,8 @@
         <v>76</v>
       </c>
       <c r="D25" s="61" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(Selected!I1)</f>
-        <v>qlPiecewiseYieldCurveData - 9th instrument (maturity: December 17th, 2014) has an invalid quote</v>
+        <f>_xll.ohRangeRetrieveError(Selected!I1)</f>
+        <v/>
       </c>
       <c r="E25" s="60"/>
       <c r="F25" s="59"/>
@@ -5004,7 +5013,7 @@
   <dimension ref="A1:N171"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -5184,9 +5193,9 @@
         <f t="shared" si="0"/>
         <v>USD_YCSTDRH_SWD</v>
       </c>
-      <c r="F5" s="14" t="e">
+      <c r="F5" s="14">
         <f>_xll.qlRateHelperQuoteValue($E5,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1.389E-3</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="13" t="b">
@@ -5301,9 +5310,9 @@
         <f t="shared" si="0"/>
         <v>USD_YCSTDRH_1MD</v>
       </c>
-      <c r="F8" s="14" t="e">
+      <c r="F8" s="14">
         <f>_xll.qlRateHelperQuoteValue($E8,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1.702E-3</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="13" t="b">
@@ -5334,9 +5343,9 @@
         <f t="shared" si="0"/>
         <v>USD_YCSTDRH_2MD</v>
       </c>
-      <c r="F9" s="14" t="e">
+      <c r="F9" s="14">
         <f>_xll.qlRateHelperQuoteValue($E9,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.0975E-3</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="13" t="b">
@@ -5367,9 +5376,9 @@
         <f t="shared" si="0"/>
         <v>USD_YCSTDRH_3MD</v>
       </c>
-      <c r="F10" s="14" t="e">
+      <c r="F10" s="14">
         <f>_xll.qlRateHelperQuoteValue($E10,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.3835000000000002E-3</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="13" t="b">
@@ -5466,9 +5475,9 @@
         <f t="shared" si="0"/>
         <v>USD_YCSTDRH_6MD</v>
       </c>
-      <c r="F13" s="14" t="e">
+      <c r="F13" s="14">
         <f>_xll.qlRateHelperQuoteValue($E13,Trigger)</f>
-        <v>#NUM!</v>
+        <v>3.5570000000000003E-3</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="13" t="b">
@@ -5664,9 +5673,9 @@
         <f t="shared" si="0"/>
         <v>USD_YCSTDRH_1YD</v>
       </c>
-      <c r="F19" s="7" t="e">
+      <c r="F19" s="7">
         <f>_xll.qlRateHelperQuoteValue($E19,Trigger)</f>
-        <v>#NUM!</v>
+        <v>6.0860000000000003E-3</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="6" t="b">
@@ -6690,8 +6699,8 @@
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E45,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H45" s="13" t="b">
-        <v>1</v>
+      <c r="H45" s="227" t="b">
+        <v>0</v>
       </c>
       <c r="I45" s="13">
         <v>60</v>
@@ -6774,8 +6783,8 @@
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E47,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H47" s="13" t="b">
-        <v>1</v>
+      <c r="H47" s="227" t="b">
+        <v>0</v>
       </c>
       <c r="I47" s="13">
         <v>60</v>
@@ -6816,8 +6825,8 @@
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E48,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H48" s="13" t="b">
-        <v>1</v>
+      <c r="H48" s="227" t="b">
+        <v>0</v>
       </c>
       <c r="I48" s="13">
         <v>60</v>
@@ -12133,9 +12142,9 @@
       <c r="H1" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="34" t="e">
+      <c r="I1" s="34">
         <f t="array" ref="I1:I126">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
-        <v>#NUM!</v>
+        <v>1.6222186172686938E-3</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -12165,8 +12174,8 @@
         <f>_xll.qlRateHelperLatestDate($D2)</f>
         <v>41656</v>
       </c>
-      <c r="I2" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I2" s="34">
+        <v>1.6222186172686938E-3</v>
       </c>
       <c r="J2" s="42"/>
       <c r="L2" s="1" t="s">
@@ -12202,8 +12211,8 @@
         <f>_xll.qlRateHelperLatestDate($D3)</f>
         <v>41659</v>
       </c>
-      <c r="I3" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I3" s="34">
+        <v>1.6222132099547131E-3</v>
       </c>
       <c r="J3" s="42"/>
       <c r="L3" s="1" t="s">
@@ -12239,12 +12248,12 @@
         <f>_xll.qlRateHelperLatestDate($D4)</f>
         <v>41660</v>
       </c>
-      <c r="I4" s="34" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J4" s="42" t="e">
+      <c r="I4" s="34">
+        <v>1.6222142914292157E-3</v>
+      </c>
+      <c r="J4" s="42">
         <f t="shared" ref="J4:J13" si="0">I4/$I$3</f>
-        <v>#NUM!</v>
+        <v>1.0000006666660683</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>115</v>
@@ -12263,9 +12272,9 @@
       <c r="D5" s="41" t="str">
         <v>USD_YCSTDRH_SWD</v>
       </c>
-      <c r="E5" s="40" t="e">
+      <c r="E5" s="40">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>#NUM!</v>
+        <v>1.389E-3</v>
       </c>
       <c r="F5" s="40">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -12279,12 +12288,12 @@
         <f>_xll.qlRateHelperLatestDate($D5)</f>
         <v>41666</v>
       </c>
-      <c r="I5" s="34" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J5" s="42" t="e">
+      <c r="I5" s="34">
+        <v>1.4860692167494509E-3</v>
+      </c>
+      <c r="J5" s="42">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>0.91607515438179488</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>116</v>
@@ -12304,9 +12313,9 @@
       <c r="D6" s="41" t="str">
         <v>USD_YCSTDRH_1MD</v>
       </c>
-      <c r="E6" s="40" t="e">
+      <c r="E6" s="40">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>#NUM!</v>
+        <v>1.702E-3</v>
       </c>
       <c r="F6" s="40">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
@@ -12320,12 +12329,12 @@
         <f>_xll.qlRateHelperLatestDate($D6)</f>
         <v>41690</v>
       </c>
-      <c r="I6" s="34" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J6" s="42" t="e">
+      <c r="I6" s="34">
+        <v>1.7137068185498574E-3</v>
+      </c>
+      <c r="J6" s="42">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>1.0564004830152374</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>117</v>
@@ -12337,7 +12346,7 @@
     <row r="7" spans="1:13" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_RateHelpersSelected#0000</v>
+        <v>USD_YCSTDRH_RateHelpersSelected#0004</v>
       </c>
       <c r="B7" s="43" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -12346,9 +12355,9 @@
       <c r="D7" s="41" t="str">
         <v>USD_YCSTDRH_2MD</v>
       </c>
-      <c r="E7" s="40" t="e">
+      <c r="E7" s="40">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>#NUM!</v>
+        <v>2.0975E-3</v>
       </c>
       <c r="F7" s="40">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -12362,12 +12371,12 @@
         <f>_xll.qlRateHelperLatestDate($D7)</f>
         <v>41718</v>
       </c>
-      <c r="I7" s="34" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J7" s="42" t="e">
+      <c r="I7" s="34">
+        <v>2.0942631220690591E-3</v>
+      </c>
+      <c r="J7" s="42">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>1.2909912884555566</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>118</v>
@@ -12380,9 +12389,9 @@
       <c r="D8" s="41" t="str">
         <v>USD_YCSTDRH_3MD</v>
       </c>
-      <c r="E8" s="40" t="e">
+      <c r="E8" s="40">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>#NUM!</v>
+        <v>2.3835000000000002E-3</v>
       </c>
       <c r="F8" s="40">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -12396,12 +12405,12 @@
         <f>_xll.qlRateHelperLatestDate($D8)</f>
         <v>41751</v>
       </c>
-      <c r="I8" s="34" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J8" s="42" t="e">
+      <c r="I8" s="34">
+        <v>2.3827994993601094E-3</v>
+      </c>
+      <c r="J8" s="42">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>1.468857166701675</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>119</v>
@@ -12414,9 +12423,9 @@
       <c r="D9" s="41" t="str">
         <v>USD_YCSTDRH_6MD</v>
       </c>
-      <c r="E9" s="40" t="e">
+      <c r="E9" s="40">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>#NUM!</v>
+        <v>3.5570000000000003E-3</v>
       </c>
       <c r="F9" s="40">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -12430,12 +12439,12 @@
         <f>_xll.qlRateHelperLatestDate($D9)</f>
         <v>41841</v>
       </c>
-      <c r="I9" s="34" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J9" s="42" t="e">
+      <c r="I9" s="34">
+        <v>3.5605629399715674E-3</v>
+      </c>
+      <c r="J9" s="42">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>2.1948797594065743</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>120</v>
@@ -12446,11 +12455,11 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D10" s="41" t="str">
-        <v>USD_YCSTDRH_FUT3MU4</v>
-      </c>
-      <c r="E10" s="40" t="e">
+        <v>USD_YCSTDRH_1YD</v>
+      </c>
+      <c r="E10" s="40">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>#NUM!</v>
+        <v>6.0860000000000003E-3</v>
       </c>
       <c r="F10" s="40">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -12458,18 +12467,18 @@
       </c>
       <c r="G10" s="12">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41899</v>
+        <v>41659</v>
       </c>
       <c r="H10" s="39">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>41990</v>
-      </c>
-      <c r="I10" s="34" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J10" s="42" t="e">
+        <v>42024</v>
+      </c>
+      <c r="I10" s="34">
+        <v>6.1024693284627857E-3</v>
+      </c>
+      <c r="J10" s="42">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>3.7618170601835668</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>121</v>
@@ -12480,11 +12489,11 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D11" s="41" t="str">
-        <v>USD_YCSTDRH_1YD</v>
-      </c>
-      <c r="E11" s="40" t="e">
+        <v>USD_YCSTDRH_FUT3MH5</v>
+      </c>
+      <c r="E11" s="40">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>#NUM!</v>
+        <v>5.6249999999999911E-3</v>
       </c>
       <c r="F11" s="40">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -12492,18 +12501,18 @@
       </c>
       <c r="G11" s="12">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41659</v>
+        <v>42081</v>
       </c>
       <c r="H11" s="39">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>42024</v>
-      </c>
-      <c r="I11" s="34" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J11" s="42" t="e">
+        <v>42173</v>
+      </c>
+      <c r="I11" s="34">
+        <v>5.9979258688212063E-3</v>
+      </c>
+      <c r="J11" s="42">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>3.6973721037499434</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>122</v>
@@ -12514,11 +12523,11 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D12" s="41" t="str">
-        <v>USD_YCSTDRH_FUT3MZ4</v>
-      </c>
-      <c r="E12" s="40" t="e">
+        <v>USD_YCSTDRH_FUT3MM5</v>
+      </c>
+      <c r="E12" s="40">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>#NUM!</v>
+        <v>7.2750000000000314E-3</v>
       </c>
       <c r="F12" s="40">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -12526,18 +12535,18 @@
       </c>
       <c r="G12" s="12">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41990</v>
+        <v>42172</v>
       </c>
       <c r="H12" s="39">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>42080</v>
-      </c>
-      <c r="I12" s="34" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J12" s="42" t="e">
+        <v>42264</v>
+      </c>
+      <c r="I12" s="34">
+        <v>6.205675240821387E-3</v>
+      </c>
+      <c r="J12" s="42">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>3.8254374965881515</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>123</v>
@@ -12548,11 +12557,11 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D13" s="41" t="str">
-        <v>USD_YCSTDRH_FUT3MH5</v>
+        <v>USD_YCSTDRH_FUT3MU5</v>
       </c>
       <c r="E13" s="40">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>5.6249999999999911E-3</v>
+        <v>9.3250000000000277E-3</v>
       </c>
       <c r="F13" s="40">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -12560,18 +12569,18 @@
       </c>
       <c r="G13" s="12">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>42081</v>
+        <v>42263</v>
       </c>
       <c r="H13" s="39">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>42173</v>
-      </c>
-      <c r="I13" s="34" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J13" s="42" t="e">
+        <v>42354</v>
+      </c>
+      <c r="I13" s="34">
+        <v>6.6251943637923201E-3</v>
+      </c>
+      <c r="J13" s="42">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>4.0840466118367225</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>124</v>
@@ -12582,11 +12591,11 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D14" s="41" t="str">
-        <v>USD_YCSTDRH_FUT3MM5</v>
+        <v>USD_YCSTDRH_FUT3MZ5</v>
       </c>
       <c r="E14" s="40">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>7.2750000000000314E-3</v>
+        <v>1.177499999999998E-2</v>
       </c>
       <c r="F14" s="40">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -12594,14 +12603,14 @@
       </c>
       <c r="G14" s="12">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>42172</v>
+        <v>42354</v>
       </c>
       <c r="H14" s="39">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>42264</v>
-      </c>
-      <c r="I14" s="34" t="e">
-        <v>#NUM!</v>
+        <v>42445</v>
+      </c>
+      <c r="I14" s="34">
+        <v>7.2351956076774143E-3</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>125</v>
@@ -12612,11 +12621,11 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D15" s="41" t="str">
-        <v>USD_YCSTDRH_FUT3MU5</v>
+        <v>USD_YCSTDRH_FUT3MH6</v>
       </c>
       <c r="E15" s="40">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>9.3250000000000277E-3</v>
+        <v>1.462500000000011E-2</v>
       </c>
       <c r="F15" s="40">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
@@ -12624,14 +12633,14 @@
       </c>
       <c r="G15" s="12">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>42263</v>
+        <v>42445</v>
       </c>
       <c r="H15" s="39">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>42354</v>
-      </c>
-      <c r="I15" s="34" t="e">
-        <v>#NUM!</v>
+        <v>42537</v>
+      </c>
+      <c r="I15" s="34">
+        <v>8.0243186383118711E-3</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>126</v>
@@ -12642,11 +12651,11 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D16" s="41" t="str">
-        <v>USD_YCSTDRH_FUT3MZ5</v>
+        <v>USD_YCSTDRH_FUT3MM6</v>
       </c>
       <c r="E16" s="40">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>1.177499999999998E-2</v>
+        <v>1.7574999999999896E-2</v>
       </c>
       <c r="F16" s="40">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
@@ -12654,14 +12663,14 @@
       </c>
       <c r="G16" s="12">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>42354</v>
+        <v>42536</v>
       </c>
       <c r="H16" s="39">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>42445</v>
-      </c>
-      <c r="I16" s="34" t="e">
-        <v>#NUM!</v>
+        <v>42628</v>
+      </c>
+      <c r="I16" s="34">
+        <v>8.9389048772908451E-3</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>127</v>
@@ -12690,8 +12699,8 @@
         <f>_xll.qlRateHelperLatestDate($D17)</f>
         <v>42755</v>
       </c>
-      <c r="I17" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I17" s="34">
+        <v>6.8936739054255049E-3</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>128</v>
@@ -12720,8 +12729,8 @@
         <f>_xll.qlRateHelperLatestDate($D18)</f>
         <v>43122</v>
       </c>
-      <c r="I18" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I18" s="34">
+        <v>1.0503721169916234E-2</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>129</v>
@@ -12750,8 +12759,8 @@
         <f>_xll.qlRateHelperLatestDate($D19)</f>
         <v>43486</v>
       </c>
-      <c r="I19" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I19" s="34">
+        <v>1.4236856473054208E-2</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>130</v>
@@ -12780,8 +12789,8 @@
         <f>_xll.qlRateHelperLatestDate($D20)</f>
         <v>43850</v>
       </c>
-      <c r="I20" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I20" s="34">
+        <v>1.7686087284873676E-2</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>131</v>
@@ -12810,8 +12819,8 @@
         <f>_xll.qlRateHelperLatestDate($D21)</f>
         <v>44216</v>
       </c>
-      <c r="I21" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I21" s="34">
+        <v>2.0631892693962907E-2</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>132</v>
@@ -12840,8 +12849,8 @@
         <f>_xll.qlRateHelperLatestDate($D22)</f>
         <v>44581</v>
       </c>
-      <c r="I22" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I22" s="34">
+        <v>2.3135785111452919E-2</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>133</v>
@@ -12870,8 +12879,8 @@
         <f>_xll.qlRateHelperLatestDate($D23)</f>
         <v>44946</v>
       </c>
-      <c r="I23" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I23" s="34">
+        <v>2.5271217555665165E-2</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>134</v>
@@ -12900,8 +12909,8 @@
         <f>_xll.qlRateHelperLatestDate($D24)</f>
         <v>45313</v>
       </c>
-      <c r="I24" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I24" s="34">
+        <v>2.7091948012482617E-2</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>135</v>
@@ -12930,8 +12939,8 @@
         <f>_xll.qlRateHelperLatestDate($D25)</f>
         <v>46042</v>
       </c>
-      <c r="I25" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I25" s="34">
+        <v>3.0079911363442038E-2</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>136</v>
@@ -12960,8 +12969,8 @@
         <f>_xll.qlRateHelperLatestDate($D26)</f>
         <v>47140</v>
       </c>
-      <c r="I26" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I26" s="34">
+        <v>3.3068736966007907E-2</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>137</v>
@@ -12990,8 +12999,8 @@
         <f>_xll.qlRateHelperLatestDate($D27)</f>
         <v>48964</v>
       </c>
-      <c r="I27" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I27" s="34">
+        <v>3.5690146581469635E-2</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>138</v>
@@ -13020,8 +13029,8 @@
         <f>_xll.qlRateHelperLatestDate($D28)</f>
         <v>50790</v>
       </c>
-      <c r="I28" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I28" s="34">
+        <v>3.6978754141574803E-2</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>139</v>
@@ -13050,8 +13059,8 @@
         <f>_xll.qlRateHelperLatestDate($D29)</f>
         <v>52616</v>
       </c>
-      <c r="I29" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I29" s="34">
+        <v>3.7621420499449887E-2</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>140</v>
@@ -13080,8 +13089,8 @@
         <f>_xll.qlRateHelperLatestDate($D30)</f>
         <v>56269</v>
       </c>
-      <c r="I30" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I30" s="34">
+        <v>3.7280444076420713E-2</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>141</v>
@@ -13110,8 +13119,8 @@
         <f>_xll.qlRateHelperLatestDate($D31)</f>
         <v>59922</v>
       </c>
-      <c r="I31" s="34" t="e">
-        <v>#NUM!</v>
+      <c r="I31" s="34">
+        <v>3.6543910739400831E-2</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>142</v>
@@ -13141,7 +13150,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I32" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.2">
@@ -13165,7 +13174,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I33" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.2">
@@ -13189,7 +13198,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I34" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.2">
@@ -13213,7 +13222,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I35" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.2">
@@ -13237,7 +13246,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I36" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.2">
@@ -13261,7 +13270,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I37" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.2">
@@ -13285,7 +13294,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I38" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.2">
@@ -13309,7 +13318,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I39" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="40" spans="4:9" x14ac:dyDescent="0.2">
@@ -13333,7 +13342,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I40" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.2">
@@ -13357,7 +13366,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I41" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.2">
@@ -13381,7 +13390,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I42" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.2">
@@ -13405,7 +13414,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I43" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.2">
@@ -13429,7 +13438,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I44" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.2">
@@ -13453,7 +13462,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I45" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.2">
@@ -13477,7 +13486,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I46" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.2">
@@ -13501,7 +13510,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I47" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.2">
@@ -13525,7 +13534,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I48" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="49" spans="4:9" x14ac:dyDescent="0.2">
@@ -13549,7 +13558,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I49" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="50" spans="4:9" x14ac:dyDescent="0.2">
@@ -13573,7 +13582,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I50" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="51" spans="4:9" x14ac:dyDescent="0.2">
@@ -13597,7 +13606,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I51" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="52" spans="4:9" x14ac:dyDescent="0.2">
@@ -13621,7 +13630,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I52" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="53" spans="4:9" x14ac:dyDescent="0.2">
@@ -13645,7 +13654,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I53" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="54" spans="4:9" x14ac:dyDescent="0.2">
@@ -13669,7 +13678,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I54" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="55" spans="4:9" x14ac:dyDescent="0.2">
@@ -13693,7 +13702,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I55" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="56" spans="4:9" x14ac:dyDescent="0.2">
@@ -13717,7 +13726,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I56" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="57" spans="4:9" x14ac:dyDescent="0.2">
@@ -13741,7 +13750,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I57" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="58" spans="4:9" x14ac:dyDescent="0.2">
@@ -13765,7 +13774,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I58" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="59" spans="4:9" x14ac:dyDescent="0.2">
@@ -13789,7 +13798,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I59" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="60" spans="4:9" x14ac:dyDescent="0.2">
@@ -13813,7 +13822,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I60" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="61" spans="4:9" x14ac:dyDescent="0.2">
@@ -13837,7 +13846,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I61" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="62" spans="4:9" x14ac:dyDescent="0.2">
@@ -13861,7 +13870,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I62" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="63" spans="4:9" x14ac:dyDescent="0.2">
@@ -13885,7 +13894,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I63" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="64" spans="4:9" x14ac:dyDescent="0.2">
@@ -13909,7 +13918,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I64" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="65" spans="4:9" x14ac:dyDescent="0.2">
@@ -13933,7 +13942,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I65" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="66" spans="4:9" x14ac:dyDescent="0.2">
@@ -13957,7 +13966,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I66" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="67" spans="4:9" x14ac:dyDescent="0.2">
@@ -13981,7 +13990,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I67" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="68" spans="4:9" x14ac:dyDescent="0.2">
@@ -14005,7 +14014,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I68" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="69" spans="4:9" x14ac:dyDescent="0.2">
@@ -14029,7 +14038,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I69" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="70" spans="4:9" x14ac:dyDescent="0.2">
@@ -14053,7 +14062,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I70" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="71" spans="4:9" x14ac:dyDescent="0.2">
@@ -14077,7 +14086,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I71" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="72" spans="4:9" x14ac:dyDescent="0.2">
@@ -14101,7 +14110,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I72" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="73" spans="4:9" x14ac:dyDescent="0.2">
@@ -14125,7 +14134,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I73" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="74" spans="4:9" x14ac:dyDescent="0.2">
@@ -14149,7 +14158,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I74" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="75" spans="4:9" x14ac:dyDescent="0.2">
@@ -14173,7 +14182,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I75" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="76" spans="4:9" x14ac:dyDescent="0.2">
@@ -14197,7 +14206,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I76" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="77" spans="4:9" x14ac:dyDescent="0.2">
@@ -14221,7 +14230,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I77" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="78" spans="4:9" x14ac:dyDescent="0.2">
@@ -14245,7 +14254,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I78" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="79" spans="4:9" x14ac:dyDescent="0.2">
@@ -14269,7 +14278,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I79" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="80" spans="4:9" x14ac:dyDescent="0.2">
@@ -14293,7 +14302,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I80" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="81" spans="4:9" x14ac:dyDescent="0.2">
@@ -14317,7 +14326,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I81" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="82" spans="4:9" x14ac:dyDescent="0.2">
@@ -14341,7 +14350,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I82" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="83" spans="4:9" x14ac:dyDescent="0.2">
@@ -14365,7 +14374,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I83" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="84" spans="4:9" x14ac:dyDescent="0.2">
@@ -14389,7 +14398,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I84" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="85" spans="4:9" x14ac:dyDescent="0.2">
@@ -14413,7 +14422,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I85" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="86" spans="4:9" x14ac:dyDescent="0.2">
@@ -14437,7 +14446,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I86" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="87" spans="4:9" x14ac:dyDescent="0.2">
@@ -14461,7 +14470,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I87" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="88" spans="4:9" x14ac:dyDescent="0.2">
@@ -14485,7 +14494,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I88" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="89" spans="4:9" x14ac:dyDescent="0.2">
@@ -14509,7 +14518,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I89" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="90" spans="4:9" x14ac:dyDescent="0.2">
@@ -14533,7 +14542,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I90" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="91" spans="4:9" x14ac:dyDescent="0.2">
@@ -14557,7 +14566,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I91" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="92" spans="4:9" x14ac:dyDescent="0.2">
@@ -14581,7 +14590,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I92" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="93" spans="4:9" x14ac:dyDescent="0.2">
@@ -14605,7 +14614,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I93" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="94" spans="4:9" x14ac:dyDescent="0.2">
@@ -14629,7 +14638,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I94" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="95" spans="4:9" x14ac:dyDescent="0.2">
@@ -14653,7 +14662,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I95" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="96" spans="4:9" x14ac:dyDescent="0.2">
@@ -14677,7 +14686,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I96" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="97" spans="4:9" x14ac:dyDescent="0.2">
@@ -14701,7 +14710,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I97" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="98" spans="4:9" x14ac:dyDescent="0.2">
@@ -14725,7 +14734,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I98" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="99" spans="4:9" x14ac:dyDescent="0.2">
@@ -14749,7 +14758,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I99" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="100" spans="4:9" x14ac:dyDescent="0.2">
@@ -14773,7 +14782,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I100" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="101" spans="4:9" x14ac:dyDescent="0.2">
@@ -14797,7 +14806,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I101" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="102" spans="4:9" x14ac:dyDescent="0.2">
@@ -14821,7 +14830,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I102" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="103" spans="4:9" x14ac:dyDescent="0.2">
@@ -14845,7 +14854,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I103" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="104" spans="4:9" x14ac:dyDescent="0.2">
@@ -14869,7 +14878,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I104" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="105" spans="4:9" x14ac:dyDescent="0.2">
@@ -14893,7 +14902,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I105" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="106" spans="4:9" x14ac:dyDescent="0.2">
@@ -14917,7 +14926,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I106" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="107" spans="4:9" x14ac:dyDescent="0.2">
@@ -14941,7 +14950,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I107" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="108" spans="4:9" x14ac:dyDescent="0.2">
@@ -14965,7 +14974,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I108" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="109" spans="4:9" x14ac:dyDescent="0.2">
@@ -14989,7 +14998,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I109" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="110" spans="4:9" x14ac:dyDescent="0.2">
@@ -15013,7 +15022,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I110" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="111" spans="4:9" x14ac:dyDescent="0.2">
@@ -15037,7 +15046,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I111" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="112" spans="4:9" x14ac:dyDescent="0.2">
@@ -15061,7 +15070,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I112" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="113" spans="4:9" x14ac:dyDescent="0.2">
@@ -15085,7 +15094,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I113" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="114" spans="4:9" x14ac:dyDescent="0.2">
@@ -15109,7 +15118,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I114" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="115" spans="4:9" x14ac:dyDescent="0.2">
@@ -15133,7 +15142,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I115" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="116" spans="4:9" x14ac:dyDescent="0.2">
@@ -15157,7 +15166,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I116" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="117" spans="4:9" x14ac:dyDescent="0.2">
@@ -15181,7 +15190,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I117" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="118" spans="4:9" x14ac:dyDescent="0.2">
@@ -15205,7 +15214,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I118" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="119" spans="4:9" x14ac:dyDescent="0.2">
@@ -15229,7 +15238,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I119" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="120" spans="4:9" x14ac:dyDescent="0.2">
@@ -15253,7 +15262,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I120" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="121" spans="4:9" x14ac:dyDescent="0.2">
@@ -15277,7 +15286,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I121" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="122" spans="4:9" x14ac:dyDescent="0.2">
@@ -15301,7 +15310,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I122" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="123" spans="4:9" x14ac:dyDescent="0.2">
@@ -15325,7 +15334,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I123" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="124" spans="4:9" x14ac:dyDescent="0.2">
@@ -15349,7 +15358,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I124" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="125" spans="4:9" x14ac:dyDescent="0.2">
@@ -15373,7 +15382,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I125" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="126" spans="4:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -15397,7 +15406,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I126" s="34" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -15420,7 +15429,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15493,7 +15504,7 @@
       </c>
       <c r="F3" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E3,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_OND#0000</v>
+        <v>USD_YCSTDRH_OND#0001</v>
       </c>
       <c r="G3" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -15520,7 +15531,7 @@
       </c>
       <c r="F4" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_SWD#0000</v>
+        <v>USD_YCSTDRH_SWD#0001</v>
       </c>
       <c r="G4" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -15547,7 +15558,7 @@
       </c>
       <c r="F5" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_2WD#0000</v>
+        <v>USD_YCSTDRH_2WD#0001</v>
       </c>
       <c r="G5" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -15574,7 +15585,7 @@
       </c>
       <c r="F6" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_3WD#0000</v>
+        <v>USD_YCSTDRH_3WD#0001</v>
       </c>
       <c r="G6" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -15601,7 +15612,7 @@
       </c>
       <c r="F7" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E7,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_1MD#0000</v>
+        <v>USD_YCSTDRH_1MD#0001</v>
       </c>
       <c r="G7" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -15628,7 +15639,7 @@
       </c>
       <c r="F8" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E8,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_2MD#0000</v>
+        <v>USD_YCSTDRH_2MD#0001</v>
       </c>
       <c r="G8" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -15655,7 +15666,7 @@
       </c>
       <c r="F9" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E9,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_3MD#0000</v>
+        <v>USD_YCSTDRH_3MD#0001</v>
       </c>
       <c r="G9" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -15682,7 +15693,7 @@
       </c>
       <c r="F10" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E10,D10,C10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_4MD#0000</v>
+        <v>USD_YCSTDRH_4MD#0001</v>
       </c>
       <c r="G10" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(F10)</f>
@@ -15709,7 +15720,7 @@
       </c>
       <c r="F11" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E11,D11,C11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_5MD#0000</v>
+        <v>USD_YCSTDRH_5MD#0001</v>
       </c>
       <c r="G11" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(F11)</f>
@@ -15736,7 +15747,7 @@
       </c>
       <c r="F12" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E12,D12,C12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_6MD#0000</v>
+        <v>USD_YCSTDRH_6MD#0001</v>
       </c>
       <c r="G12" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(F12)</f>
@@ -15763,7 +15774,7 @@
       </c>
       <c r="F13" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E13,D13,C13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_7MD#0000</v>
+        <v>USD_YCSTDRH_7MD#0001</v>
       </c>
       <c r="G13" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(F13)</f>
@@ -15790,7 +15801,7 @@
       </c>
       <c r="F14" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E14,D14,C14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_8MD#0000</v>
+        <v>USD_YCSTDRH_8MD#0001</v>
       </c>
       <c r="G14" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(F14)</f>
@@ -15817,7 +15828,7 @@
       </c>
       <c r="F15" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E15,D15,C15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_9MD#0000</v>
+        <v>USD_YCSTDRH_9MD#0001</v>
       </c>
       <c r="G15" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(F15)</f>
@@ -15844,7 +15855,7 @@
       </c>
       <c r="F16" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E16,D16,C16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_10MD#0000</v>
+        <v>USD_YCSTDRH_10MD#0001</v>
       </c>
       <c r="G16" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(F16)</f>
@@ -15871,7 +15882,7 @@
       </c>
       <c r="F17" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E17,D17,C17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_11MD#0000</v>
+        <v>USD_YCSTDRH_11MD#0001</v>
       </c>
       <c r="G17" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(F17)</f>
@@ -15898,7 +15909,7 @@
       </c>
       <c r="F18" s="171" t="str">
         <f>_xll.qlDepositRateHelper(E18,D18,C18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_1YD#0000</v>
+        <v>USD_YCSTDRH_1YD#0001</v>
       </c>
       <c r="G18" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(F18)</f>
@@ -16011,7 +16022,7 @@
       </c>
       <c r="H3" s="109" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_TND#0000</v>
+        <v>USD_YCSTDRH_TND#0001</v>
       </c>
       <c r="I3" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -16043,7 +16054,7 @@
       </c>
       <c r="H4" s="104" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_SND#0000</v>
+        <v>USD_YCSTDRH_SND#0001</v>
       </c>
       <c r="I4" s="103" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -16181,7 +16192,7 @@
       </c>
       <c r="I3" s="155" t="str">
         <f>_xll.qlFuturesRateHelper(H3,$F3,$D3,$E3,$G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MG4#0000</v>
+        <v>USD_YCSTDRH_FUT3MG4#0001</v>
       </c>
       <c r="J3" s="154" t="str">
         <f>_xll.ohRangeRetrieveError(I3)</f>
@@ -16219,7 +16230,7 @@
       </c>
       <c r="I4" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H4,$F4,$D4,$E4,$G4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MH4#0000</v>
+        <v>USD_YCSTDRH_FUT3MH4#0001</v>
       </c>
       <c r="J4" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I4)</f>
@@ -16257,7 +16268,7 @@
       </c>
       <c r="I5" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H5,$F5,$D5,$E5,$G5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MJ4#0000</v>
+        <v>USD_YCSTDRH_FUT3MJ4#0001</v>
       </c>
       <c r="J5" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I5)</f>
@@ -16295,7 +16306,7 @@
       </c>
       <c r="I6" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H6,$F6,$D6,$E6,$G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MK4#0000</v>
+        <v>USD_YCSTDRH_FUT3MK4#0001</v>
       </c>
       <c r="J6" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I6)</f>
@@ -16333,7 +16344,7 @@
       </c>
       <c r="I7" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H7,$F7,$D7,$E7,$G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MM4#0000</v>
+        <v>USD_YCSTDRH_FUT3MM4#0001</v>
       </c>
       <c r="J7" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I7)</f>
@@ -16371,7 +16382,7 @@
       </c>
       <c r="I8" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H8,$F8,$D8,$E8,$G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MN4#0000</v>
+        <v>USD_YCSTDRH_FUT3MN4#0001</v>
       </c>
       <c r="J8" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I8)</f>
@@ -16409,7 +16420,7 @@
       </c>
       <c r="I9" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H9,$F9,$D9,$E9,$G9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MQ4#0000</v>
+        <v>USD_YCSTDRH_FUT3MQ4#0001</v>
       </c>
       <c r="J9" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
@@ -16447,7 +16458,7 @@
       </c>
       <c r="I10" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H10,$F10,$D10,$E10,$G10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MU4#0000</v>
+        <v>USD_YCSTDRH_FUT3MU4#0001</v>
       </c>
       <c r="J10" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
@@ -16485,7 +16496,7 @@
       </c>
       <c r="I11" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H11,$F11,$D11,$E11,$G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MV4#0000</v>
+        <v>USD_YCSTDRH_FUT3MV4#0001</v>
       </c>
       <c r="J11" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I11)</f>
@@ -16523,7 +16534,7 @@
       </c>
       <c r="I12" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H12,$F12,$D12,$E12,$G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MX4#0000</v>
+        <v>USD_YCSTDRH_FUT3MX4#0001</v>
       </c>
       <c r="J12" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I12)</f>
@@ -16561,7 +16572,7 @@
       </c>
       <c r="I13" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H13,$F13,$D13,$E13,$G13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MZ4#0000</v>
+        <v>USD_YCSTDRH_FUT3MZ4#0001</v>
       </c>
       <c r="J13" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I13)</f>
@@ -16599,7 +16610,7 @@
       </c>
       <c r="I14" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H14,$F14,$D14,$E14,$G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MF5#0000</v>
+        <v>USD_YCSTDRH_FUT3MF5#0001</v>
       </c>
       <c r="J14" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I14)</f>
@@ -16675,7 +16686,7 @@
       </c>
       <c r="I16" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H16,$F16,$D16,$E16,$G16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MH5#0000</v>
+        <v>USD_YCSTDRH_FUT3MH5#0001</v>
       </c>
       <c r="J16" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I16)</f>
@@ -16789,7 +16800,7 @@
       </c>
       <c r="I19" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H19,$F19,$D19,$E19,$G19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MM5#0000</v>
+        <v>USD_YCSTDRH_FUT3MM5#0001</v>
       </c>
       <c r="J19" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I19)</f>
@@ -16903,7 +16914,7 @@
       </c>
       <c r="I22" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H22,$F22,$D22,$E22,$G22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MU5#0000</v>
+        <v>USD_YCSTDRH_FUT3MU5#0001</v>
       </c>
       <c r="J22" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I22)</f>
@@ -17017,7 +17028,7 @@
       </c>
       <c r="I25" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H25,$F25,$D25,$E25,$G25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MZ5#0000</v>
+        <v>USD_YCSTDRH_FUT3MZ5#0001</v>
       </c>
       <c r="J25" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I25)</f>
@@ -17131,7 +17142,7 @@
       </c>
       <c r="I28" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H28,$F28,$D28,$E28,$G28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MH6#0000</v>
+        <v>USD_YCSTDRH_FUT3MH6#0001</v>
       </c>
       <c r="J28" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I28)</f>
@@ -17245,7 +17256,7 @@
       </c>
       <c r="I31" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H31,$F31,$D31,$E31,$G31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MM6#0000</v>
+        <v>USD_YCSTDRH_FUT3MM6#0001</v>
       </c>
       <c r="J31" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I31)</f>
@@ -17359,7 +17370,7 @@
       </c>
       <c r="I34" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H34,$F34,$D34,$E34,$G34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MU6#0000</v>
+        <v>USD_YCSTDRH_FUT3MU6#0001</v>
       </c>
       <c r="J34" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I34)</f>
@@ -17473,7 +17484,7 @@
       </c>
       <c r="I37" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H37,$F37,$D37,$E37,$G37,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MZ6#0000</v>
+        <v>USD_YCSTDRH_FUT3MZ6#0001</v>
       </c>
       <c r="J37" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I37)</f>
@@ -17587,7 +17598,7 @@
       </c>
       <c r="I40" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H40,$F40,$D40,$E40,$G40,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MH7#0000</v>
+        <v>USD_YCSTDRH_FUT3MH7#0001</v>
       </c>
       <c r="J40" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I40)</f>
@@ -17698,7 +17709,7 @@
       </c>
       <c r="I43" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H43,$F43,$D43,$E43,$G43,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MM7#0000</v>
+        <v>USD_YCSTDRH_FUT3MM7#0001</v>
       </c>
       <c r="J43" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I43)</f>
@@ -17809,7 +17820,7 @@
       </c>
       <c r="I46" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H46,$F46,$D46,$E46,$G46,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MU7#0000</v>
+        <v>USD_YCSTDRH_FUT3MU7#0001</v>
       </c>
       <c r="J46" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I46)</f>
@@ -17920,7 +17931,7 @@
       </c>
       <c r="I49" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H49,$F49,$D49,$E49,$G49,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MZ7#0000</v>
+        <v>USD_YCSTDRH_FUT3MZ7#0001</v>
       </c>
       <c r="J49" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I49)</f>
@@ -18031,7 +18042,7 @@
       </c>
       <c r="I52" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H52,$F52,$D52,$E52,$G52,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MH8#0000</v>
+        <v>USD_YCSTDRH_FUT3MH8#0001</v>
       </c>
       <c r="J52" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I52)</f>
@@ -18142,7 +18153,7 @@
       </c>
       <c r="I55" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H55,$F55,$D55,$E55,$G55,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MM8#0000</v>
+        <v>USD_YCSTDRH_FUT3MM8#0001</v>
       </c>
       <c r="J55" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I55)</f>
@@ -18253,7 +18264,7 @@
       </c>
       <c r="I58" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H58,$F58,$D58,$E58,$G58,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MU8#0000</v>
+        <v>USD_YCSTDRH_FUT3MU8#0001</v>
       </c>
       <c r="J58" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I58)</f>
@@ -18364,7 +18375,7 @@
       </c>
       <c r="I61" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H61,$F61,$D61,$E61,$G61,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MZ8#0000</v>
+        <v>USD_YCSTDRH_FUT3MZ8#0001</v>
       </c>
       <c r="J61" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I61)</f>
@@ -18475,7 +18486,7 @@
       </c>
       <c r="I64" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H64,$F64,$D64,$E64,$G64,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MH9#0000</v>
+        <v>USD_YCSTDRH_FUT3MH9#0001</v>
       </c>
       <c r="J64" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I64)</f>
@@ -18586,7 +18597,7 @@
       </c>
       <c r="I67" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H67,$F67,$D67,$E67,$G67,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MM9#0000</v>
+        <v>USD_YCSTDRH_FUT3MM9#0001</v>
       </c>
       <c r="J67" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I67)</f>
@@ -18697,7 +18708,7 @@
       </c>
       <c r="I70" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H70,$F70,$D70,$E70,$G70,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MU9#0000</v>
+        <v>USD_YCSTDRH_FUT3MU9#0001</v>
       </c>
       <c r="J70" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I70)</f>
@@ -18808,7 +18819,7 @@
       </c>
       <c r="I73" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H73,$F73,$D73,$E73,$G73,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MZ9#0000</v>
+        <v>USD_YCSTDRH_FUT3MZ9#0001</v>
       </c>
       <c r="J73" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I73)</f>
@@ -18919,7 +18930,7 @@
       </c>
       <c r="I76" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H76,$F76,$D76,$E76,$G76,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MH0#0000</v>
+        <v>USD_YCSTDRH_FUT3MH0#0001</v>
       </c>
       <c r="J76" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I76)</f>
@@ -19030,7 +19041,7 @@
       </c>
       <c r="I79" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H79,$F79,$D79,$E79,$G79,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MM0#0000</v>
+        <v>USD_YCSTDRH_FUT3MM0#0001</v>
       </c>
       <c r="J79" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I79)</f>
@@ -19141,7 +19152,7 @@
       </c>
       <c r="I82" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H82,$F82,$D82,$E82,$G82,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MU0#0000</v>
+        <v>USD_YCSTDRH_FUT3MU0#0001</v>
       </c>
       <c r="J82" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I82)</f>
@@ -19252,7 +19263,7 @@
       </c>
       <c r="I85" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H85,$F85,$D85,$E85,$G85,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MZ0#0000</v>
+        <v>USD_YCSTDRH_FUT3MZ0#0001</v>
       </c>
       <c r="J85" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I85)</f>
@@ -19363,7 +19374,7 @@
       </c>
       <c r="I88" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H88,$F88,$D88,$E88,$G88,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MH1#0000</v>
+        <v>USD_YCSTDRH_FUT3MH1#0001</v>
       </c>
       <c r="J88" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I88)</f>
@@ -19474,7 +19485,7 @@
       </c>
       <c r="I91" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H91,$F91,$D91,$E91,$G91,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MM1#0000</v>
+        <v>USD_YCSTDRH_FUT3MM1#0001</v>
       </c>
       <c r="J91" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I91)</f>
@@ -19585,7 +19596,7 @@
       </c>
       <c r="I94" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H94,$F94,$D94,$E94,$G94,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MU1#0000</v>
+        <v>USD_YCSTDRH_FUT3MU1#0001</v>
       </c>
       <c r="J94" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I94)</f>
@@ -19696,7 +19707,7 @@
       </c>
       <c r="I97" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H97,$F97,$D97,$E97,$G97,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MZ1#0000</v>
+        <v>USD_YCSTDRH_FUT3MZ1#0001</v>
       </c>
       <c r="J97" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I97)</f>
@@ -19807,7 +19818,7 @@
       </c>
       <c r="I100" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H100,$F100,$D100,$E100,$G100,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MH2#0000</v>
+        <v>USD_YCSTDRH_FUT3MH2#0001</v>
       </c>
       <c r="J100" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I100)</f>
@@ -19918,7 +19929,7 @@
       </c>
       <c r="I103" s="147" t="str">
         <f>_xll.qlFuturesRateHelper(H103,$F103,$D103,$E103,$G103,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_FUT3MM2#0000</v>
+        <v>USD_YCSTDRH_FUT3MM2#0001</v>
       </c>
       <c r="J103" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(I103)</f>
@@ -20774,7 +20785,7 @@
       </c>
       <c r="L4" s="211" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>USD_YCSTDRH_AM3L_Libor6M#0000</v>
+        <v>USD_YCSTDRH_AM3L_Libor6M#0001</v>
       </c>
       <c r="M4" s="210" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -20838,7 +20849,7 @@
       </c>
       <c r="L6" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L1Y#0000</v>
+        <v>USD_YCSTDRH_AM3L1Y#0001</v>
       </c>
       <c r="M6" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -20889,7 +20900,7 @@
       </c>
       <c r="L7" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L15M#0000</v>
+        <v>USD_YCSTDRH_AM3L15M#0001</v>
       </c>
       <c r="M7" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -20944,7 +20955,7 @@
       </c>
       <c r="L8" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L18M#0000</v>
+        <v>USD_YCSTDRH_AM3L18M#0001</v>
       </c>
       <c r="M8" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -20999,7 +21010,7 @@
       </c>
       <c r="L9" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L21M#0000</v>
+        <v>USD_YCSTDRH_AM3L21M#0001</v>
       </c>
       <c r="M9" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -21050,7 +21061,7 @@
       </c>
       <c r="L10" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L2Y#0000</v>
+        <v>USD_YCSTDRH_AM3L2Y#0001</v>
       </c>
       <c r="M10" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -21105,7 +21116,7 @@
       </c>
       <c r="L11" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L3Y#0000</v>
+        <v>USD_YCSTDRH_AM3L3Y#0001</v>
       </c>
       <c r="M11" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -21151,7 +21162,7 @@
       </c>
       <c r="L12" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L4Y#0000</v>
+        <v>USD_YCSTDRH_AM3L4Y#0001</v>
       </c>
       <c r="M12" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -21197,7 +21208,7 @@
       </c>
       <c r="L13" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L5Y#0000</v>
+        <v>USD_YCSTDRH_AM3L5Y#0001</v>
       </c>
       <c r="M13" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -21243,7 +21254,7 @@
       </c>
       <c r="L14" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L6Y#0000</v>
+        <v>USD_YCSTDRH_AM3L6Y#0001</v>
       </c>
       <c r="M14" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -21289,7 +21300,7 @@
       </c>
       <c r="L15" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L7Y#0000</v>
+        <v>USD_YCSTDRH_AM3L7Y#0001</v>
       </c>
       <c r="M15" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -21335,7 +21346,7 @@
       </c>
       <c r="L16" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L8Y#0000</v>
+        <v>USD_YCSTDRH_AM3L8Y#0001</v>
       </c>
       <c r="M16" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -21381,7 +21392,7 @@
       </c>
       <c r="L17" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L9Y#0000</v>
+        <v>USD_YCSTDRH_AM3L9Y#0001</v>
       </c>
       <c r="M17" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -21427,7 +21438,7 @@
       </c>
       <c r="L18" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L10Y#0000</v>
+        <v>USD_YCSTDRH_AM3L10Y#0001</v>
       </c>
       <c r="M18" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -21473,7 +21484,7 @@
       </c>
       <c r="L19" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L11Y#0000</v>
+        <v>USD_YCSTDRH_AM3L11Y#0001</v>
       </c>
       <c r="M19" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -21519,7 +21530,7 @@
       </c>
       <c r="L20" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L12Y#0000</v>
+        <v>USD_YCSTDRH_AM3L12Y#0001</v>
       </c>
       <c r="M20" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -21565,7 +21576,7 @@
       </c>
       <c r="L21" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L13Y#0000</v>
+        <v>USD_YCSTDRH_AM3L13Y#0001</v>
       </c>
       <c r="M21" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -21611,7 +21622,7 @@
       </c>
       <c r="L22" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L14Y#0000</v>
+        <v>USD_YCSTDRH_AM3L14Y#0001</v>
       </c>
       <c r="M22" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -21657,7 +21668,7 @@
       </c>
       <c r="L23" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L15Y#0000</v>
+        <v>USD_YCSTDRH_AM3L15Y#0001</v>
       </c>
       <c r="M23" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -21703,7 +21714,7 @@
       </c>
       <c r="L24" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L16Y#0000</v>
+        <v>USD_YCSTDRH_AM3L16Y#0001</v>
       </c>
       <c r="M24" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -21749,7 +21760,7 @@
       </c>
       <c r="L25" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L17Y#0000</v>
+        <v>USD_YCSTDRH_AM3L17Y#0001</v>
       </c>
       <c r="M25" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -21795,7 +21806,7 @@
       </c>
       <c r="L26" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L18Y#0000</v>
+        <v>USD_YCSTDRH_AM3L18Y#0001</v>
       </c>
       <c r="M26" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -21841,7 +21852,7 @@
       </c>
       <c r="L27" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L19Y#0000</v>
+        <v>USD_YCSTDRH_AM3L19Y#0001</v>
       </c>
       <c r="M27" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -21887,7 +21898,7 @@
       </c>
       <c r="L28" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L20Y#0000</v>
+        <v>USD_YCSTDRH_AM3L20Y#0001</v>
       </c>
       <c r="M28" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -21933,7 +21944,7 @@
       </c>
       <c r="L29" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L21Y#0000</v>
+        <v>USD_YCSTDRH_AM3L21Y#0001</v>
       </c>
       <c r="M29" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -21979,7 +21990,7 @@
       </c>
       <c r="L30" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L22Y#0000</v>
+        <v>USD_YCSTDRH_AM3L22Y#0001</v>
       </c>
       <c r="M30" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -22025,7 +22036,7 @@
       </c>
       <c r="L31" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L23Y#0000</v>
+        <v>USD_YCSTDRH_AM3L23Y#0001</v>
       </c>
       <c r="M31" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -22071,7 +22082,7 @@
       </c>
       <c r="L32" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L24Y#0000</v>
+        <v>USD_YCSTDRH_AM3L24Y#0001</v>
       </c>
       <c r="M32" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -22117,7 +22128,7 @@
       </c>
       <c r="L33" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L25Y#0000</v>
+        <v>USD_YCSTDRH_AM3L25Y#0001</v>
       </c>
       <c r="M33" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -22163,7 +22174,7 @@
       </c>
       <c r="L34" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L26Y#0000</v>
+        <v>USD_YCSTDRH_AM3L26Y#0001</v>
       </c>
       <c r="M34" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -22209,7 +22220,7 @@
       </c>
       <c r="L35" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L27Y#0000</v>
+        <v>USD_YCSTDRH_AM3L27Y#0001</v>
       </c>
       <c r="M35" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -22255,7 +22266,7 @@
       </c>
       <c r="L36" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L28Y#0000</v>
+        <v>USD_YCSTDRH_AM3L28Y#0001</v>
       </c>
       <c r="M36" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -22301,7 +22312,7 @@
       </c>
       <c r="L37" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L29Y#0000</v>
+        <v>USD_YCSTDRH_AM3L29Y#0001</v>
       </c>
       <c r="M37" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -22347,7 +22358,7 @@
       </c>
       <c r="L38" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L30Y#0000</v>
+        <v>USD_YCSTDRH_AM3L30Y#0001</v>
       </c>
       <c r="M38" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -22393,7 +22404,7 @@
       </c>
       <c r="L39" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L35Y#0000</v>
+        <v>USD_YCSTDRH_AM3L35Y#0001</v>
       </c>
       <c r="M39" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -22439,7 +22450,7 @@
       </c>
       <c r="L40" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L40Y#0000</v>
+        <v>USD_YCSTDRH_AM3L40Y#0001</v>
       </c>
       <c r="M40" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -22485,7 +22496,7 @@
       </c>
       <c r="L41" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L50Y#0000</v>
+        <v>USD_YCSTDRH_AM3L50Y#0001</v>
       </c>
       <c r="M41" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -22531,7 +22542,7 @@
       </c>
       <c r="L42" s="193" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCSTDRH_AM3L60Y#0000</v>
+        <v>USD_YCSTDRH_AM3L60Y#0001</v>
       </c>
       <c r="M42" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>

</xml_diff>